<commit_message>
Add a unicode char to example files
</commit_message>
<xml_diff>
--- a/test/example.xlsx
+++ b/test/example.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">C1</t>
   </si>
   <si>
-    <t xml:space="preserve">1uF 0603 X5R</t>
+    <t xml:space="preserve">1μF 0603 X5R</t>
   </si>
   <si>
     <t xml:space="preserve">Murata</t>
@@ -268,6 +268,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -352,12 +353,12 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix retailer column dash replacing, add some tests
</commit_message>
<xml_diff>
--- a/test/example.xlsx
+++ b/test/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="81">
   <si>
     <t xml:space="preserve">References</t>
   </si>
@@ -67,6 +67,9 @@
     <t xml:space="preserve">490-3290-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">624-2496</t>
+  </si>
+  <si>
     <t xml:space="preserve">91R0949</t>
   </si>
   <si>
@@ -88,6 +91,9 @@
     <t xml:space="preserve">06036D106MAT2A</t>
   </si>
   <si>
+    <t xml:space="preserve">788-2893</t>
+  </si>
+  <si>
     <t xml:space="preserve">04X3239</t>
   </si>
   <si>
@@ -119,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">LL4148FSCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">670-8826</t>
   </si>
   <si>
     <t xml:space="preserve">14M6003</t>
@@ -353,13 +362,10 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -415,11 +421,11 @@
       <c r="G2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>6242496</v>
+      <c r="H2" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>1828900</v>
@@ -427,31 +433,31 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>7882893</v>
+        <v>22</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>2211164</v>
@@ -459,31 +465,31 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>8015347</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>1288255</v>
@@ -491,28 +497,28 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>6708826</v>
+        <v>33</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>35</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>7355513</v>
@@ -520,31 +526,31 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>7008023</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>1465989</v>
@@ -552,31 +558,31 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>5429377</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>2468006</v>
@@ -584,31 +590,31 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>8206928</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>1469749</v>
@@ -616,31 +622,31 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>8206916</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>1692517</v>
@@ -648,31 +654,31 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>8280617</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>1652871</v>
@@ -680,31 +686,31 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>6183583</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>9237496</v>
@@ -712,19 +718,19 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>214375657</v>
@@ -733,7 +739,7 @@
         <v>4791491</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>3801287</v>

</xml_diff>